<commit_message>
update predictions notebook, add notebook with param tuning for LGBM models, add notebook to visualize correlations
</commit_message>
<xml_diff>
--- a/MAE_assessment_NHL.xlsx
+++ b/MAE_assessment_NHL.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\machine_learning\DFS\NHL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566718A-88E3-4DE5-9628-761F2C6E1B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72D298-C472-493D-88C9-2652BB79D36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21210" yWindow="3165" windowWidth="15300" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10095" yWindow="1785" windowWidth="26250" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RF models" sheetId="1" r:id="rId1"/>
-    <sheet name="LGBM models" sheetId="3" r:id="rId2"/>
+    <sheet name="LGBM models" sheetId="3" r:id="rId1"/>
+    <sheet name="RF models" sheetId="1" r:id="rId2"/>
+    <sheet name="TF models" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>Position</t>
   </si>
@@ -55,9 +56,6 @@
     <t>n_estimators</t>
   </si>
   <si>
-    <t>parameters tuned on all features model</t>
-  </si>
-  <si>
     <t>parameters tuned on each model</t>
   </si>
   <si>
@@ -68,6 +66,9 @@
   </si>
   <si>
     <t>no parameter tuning</t>
+  </si>
+  <si>
+    <t>MAE (corr)</t>
   </si>
 </sst>
 </file>
@@ -393,10 +394,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09AD4BE-3680-45BD-B67D-B39DA6570F23}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5.86</v>
+      </c>
+      <c r="C3">
+        <v>5.86</v>
+      </c>
+      <c r="D3">
+        <v>5.87</v>
+      </c>
+      <c r="E3">
+        <v>5.88</v>
+      </c>
+      <c r="F3">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>5.81</v>
+      </c>
+      <c r="C4">
+        <v>5.81</v>
+      </c>
+      <c r="D4">
+        <v>5.82</v>
+      </c>
+      <c r="E4">
+        <v>5.83</v>
+      </c>
+      <c r="F4">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="C5">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D5">
+        <v>4.37</v>
+      </c>
+      <c r="E5">
+        <v>4.37</v>
+      </c>
+      <c r="F5">
+        <v>4.37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>9.67</v>
+      </c>
+      <c r="C6">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="D6">
+        <v>9.74</v>
+      </c>
+      <c r="E6">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="F6">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>5.85</v>
+      </c>
+      <c r="C10">
+        <v>5.85</v>
+      </c>
+      <c r="D10">
+        <v>5.85</v>
+      </c>
+      <c r="E10">
+        <v>5.86</v>
+      </c>
+      <c r="F10">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5.81</v>
+      </c>
+      <c r="C11">
+        <v>5.81</v>
+      </c>
+      <c r="D11">
+        <v>5.82</v>
+      </c>
+      <c r="E11">
+        <v>5.82</v>
+      </c>
+      <c r="F11">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="C12">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D12">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E12">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F12">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="C13">
+        <v>9.61</v>
+      </c>
+      <c r="D13">
+        <v>9.75</v>
+      </c>
+      <c r="E13">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="F13">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -453,7 +688,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -476,7 +711,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -525,19 +760,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09AD4BE-3680-45BD-B67D-B39DA6570F23}">
-  <dimension ref="A1:F20"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8940D254-DE31-4D0E-A2A1-133EDF2CB5FC}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="B3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,187 +786,47 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>5.86</v>
-      </c>
-      <c r="C3">
-        <v>5.86</v>
-      </c>
-      <c r="D3">
-        <v>5.87</v>
-      </c>
-      <c r="E3">
-        <v>5.88</v>
-      </c>
-      <c r="F3">
-        <v>5.88</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>5.81</v>
-      </c>
-      <c r="C4">
-        <v>5.81</v>
-      </c>
-      <c r="D4">
-        <v>5.82</v>
-      </c>
-      <c r="E4">
-        <v>5.83</v>
-      </c>
-      <c r="F4">
-        <v>5.83</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="C5">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="D5">
-        <v>4.37</v>
-      </c>
-      <c r="E5">
-        <v>4.37</v>
-      </c>
-      <c r="F5">
-        <v>4.37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>9.67</v>
-      </c>
-      <c r="C6">
-        <v>9.7200000000000006</v>
-      </c>
-      <c r="D6">
-        <v>9.74</v>
-      </c>
-      <c r="E6">
-        <v>9.7799999999999994</v>
-      </c>
-      <c r="F6">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>